<commit_message>
scripts updated (Adrian v1.8)
</commit_message>
<xml_diff>
--- a/IMP_X_FDR/Resources/libraries/support_peplib1.xlsx
+++ b/IMP_X_FDR/Resources/libraries/support_peplib1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian.vasiu\Desktop\biopython-software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian.vasiu\Desktop\florian code allmost compatible\local_software_3\v1.4\Resources\libraries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307F61DE-6488-4D83-9028-5E5A81CC2C05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BF4824-A57C-4A5D-8DAC-CF3D9CEC57D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="7950" yWindow="8985" windowWidth="17280" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +418,12 @@
       <color rgb="FFDD0055"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -440,9 +446,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +733,7 @@
   <dimension ref="A1:E222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +753,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>5</v>
       </c>
       <c r="E2" s="1"/>

</xml_diff>